<commit_message>
case9. Generator status updated.
</commit_message>
<xml_diff>
--- a/data/CS5/case9/case9_2044.xlsx
+++ b/data/CS5/case9/case9_2044.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resources-planning-no_esso-degradation\data\CS5\case9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1997EBD8-D327-47EE-A587-62E354EAD306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB85BF2F-5EC2-4181-BC94-17E93D0CE437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34200" yWindow="-8880" windowWidth="28800" windowHeight="15285" tabRatio="722" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31140" yWindow="-11655" windowWidth="17280" windowHeight="9960" tabRatio="722" firstSheet="79" activeTab="82" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -4400,7 +4400,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:K1"/>
     </sheetView>
   </sheetViews>
@@ -31062,7 +31062,7 @@
   <dimension ref="A1:Y10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U43" sqref="U43"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -65669,7 +65669,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49630D89-783A-49F7-9E51-4F1FD5546230}">
   <dimension ref="A1:Y10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>

</xml_diff>